<commit_message>
Added code that inserts a zero-width space before leading zeroes, to ensure that excel doesn't remove the leading zero.
</commit_message>
<xml_diff>
--- a/processed_ICD_codes/Schnitzer_et_al_2011_ICD_crossmapping_for_appendix_with_codes_and_descriptions.xlsx
+++ b/processed_ICD_codes/Schnitzer_et_al_2011_ICD_crossmapping_for_appendix_with_codes_and_descriptions.xlsx
@@ -89,7 +89,7 @@
     <t xml:space="preserve">V71.81</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
+    <t xml:space="preserve">N/A</t>
   </si>
   <si>
     <t xml:space="preserve">No ICD-9 code for Observation for abuse/neglect</t>
@@ -500,13 +500,13 @@
     <t xml:space="preserve">comments_icd9</t>
   </si>
   <si>
-    <t xml:space="preserve">icd_10</t>
-  </si>
-  <si>
     <t xml:space="preserve">comments_icd10</t>
   </si>
   <si>
     <t xml:space="preserve">767</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">P10-P15,P52.4,P52.6,P52.8,P52.9</t>
@@ -2485,264 +2485,1378 @@
         <v>159</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>161</v>
-      </c>
-      <c r="F1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>163</v>
+      <c r="B2" t="n">
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2"/>
+        <v>162</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
       <c r="E2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" t="s">
         <v>164</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>166</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3"/>
+        <v>162</v>
+      </c>
+      <c r="D3" t="s">
+        <v>162</v>
+      </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>168</v>
+        <v>164</v>
+      </c>
+      <c r="G3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>169</v>
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F4"/>
+        <v>163</v>
+      </c>
+      <c r="F4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>173</v>
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5"/>
+        <v>162</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
       <c r="E5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5"/>
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>175</v>
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6"/>
+        <v>162</v>
+      </c>
+      <c r="D6" t="s">
+        <v>162</v>
+      </c>
       <c r="E6" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6"/>
+        <v>163</v>
+      </c>
+      <c r="F6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>177</v>
+        <v>2</v>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F7"/>
+        <v>163</v>
+      </c>
+      <c r="F7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>181</v>
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D8"/>
+        <v>166</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>167</v>
+      </c>
+      <c r="G8" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>184</v>
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D9"/>
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
+        <v>166</v>
+      </c>
       <c r="E9" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>167</v>
+      </c>
+      <c r="G9" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>187</v>
+        <v>2</v>
+      </c>
+      <c r="B10" t="n">
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10"/>
+        <v>166</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
       <c r="E10" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10"/>
+        <v>163</v>
+      </c>
+      <c r="F10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>189</v>
+        <v>2</v>
+      </c>
+      <c r="B11" t="n">
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
-      </c>
-      <c r="D11"/>
+        <v>166</v>
+      </c>
+      <c r="D11" t="s">
+        <v>166</v>
+      </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>191</v>
+        <v>167</v>
+      </c>
+      <c r="G11" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>192</v>
+        <v>3</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D12"/>
+        <v>169</v>
+      </c>
+      <c r="D12" t="s">
+        <v>170</v>
+      </c>
       <c r="E12" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>172</v>
+      </c>
+      <c r="G12" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>195</v>
+        <v>4</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13"/>
+        <v>173</v>
+      </c>
+      <c r="D13" t="s">
+        <v>173</v>
+      </c>
       <c r="E13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F13"/>
+        <v>163</v>
+      </c>
+      <c r="F13" t="s">
+        <v>174</v>
+      </c>
+      <c r="G13" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>197</v>
+        <v>5</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>201</v>
+        <v>176</v>
+      </c>
+      <c r="G14" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>6</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" t="n">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" t="s">
+        <v>178</v>
+      </c>
+      <c r="E19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F19" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>7</v>
+      </c>
+      <c r="B20" t="n">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>7</v>
+      </c>
+      <c r="B21" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>7</v>
+      </c>
+      <c r="B22" t="n">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" t="n">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>8</v>
+      </c>
+      <c r="B24" t="n">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" t="s">
+        <v>185</v>
+      </c>
+      <c r="G24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>8</v>
+      </c>
+      <c r="B25" t="n">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" t="s">
+        <v>185</v>
+      </c>
+      <c r="G25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>9</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>187</v>
+      </c>
+      <c r="D26" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" t="n">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>9</v>
+      </c>
+      <c r="B28" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>9</v>
+      </c>
+      <c r="B29" t="n">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>187</v>
+      </c>
+      <c r="D29" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>9</v>
+      </c>
+      <c r="B30" t="n">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F31" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>10</v>
+      </c>
+      <c r="B32" t="n">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F32" t="s">
+        <v>190</v>
+      </c>
+      <c r="G32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>11</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>11</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" t="s">
+        <v>193</v>
+      </c>
+      <c r="G34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>11</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" t="s">
+        <v>192</v>
+      </c>
+      <c r="E35" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" t="s">
+        <v>193</v>
+      </c>
+      <c r="G35" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>11</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D36" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+      <c r="G36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>12</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E37" t="s">
+        <v>163</v>
+      </c>
+      <c r="F37" t="s">
+        <v>196</v>
+      </c>
+      <c r="G37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>13</v>
+      </c>
+      <c r="B38" t="n">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" t="s">
+        <v>198</v>
+      </c>
+      <c r="E38" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>13</v>
+      </c>
+      <c r="B39" t="n">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>197</v>
+      </c>
+      <c r="D39" t="s">
+        <v>198</v>
+      </c>
+      <c r="E39" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>13</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" t="s">
+        <v>198</v>
+      </c>
+      <c r="E40" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>13</v>
+      </c>
+      <c r="B41" t="n">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" t="s">
+        <v>199</v>
+      </c>
+      <c r="F41" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>13</v>
+      </c>
+      <c r="B42" t="n">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E42" t="s">
+        <v>199</v>
+      </c>
+      <c r="F42" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>14</v>
+      </c>
+      <c r="B43" t="n">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>202</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D43" t="s">
         <v>202</v>
       </c>
-      <c r="D15"/>
-      <c r="E15" t="s">
+      <c r="E43" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" t="s">
         <v>203</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G43" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>14</v>
+      </c>
+      <c r="B44" t="n">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" t="s">
+        <v>202</v>
+      </c>
+      <c r="E44" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" t="s">
+        <v>203</v>
+      </c>
+      <c r="G44" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>14</v>
+      </c>
+      <c r="B45" t="n">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>202</v>
+      </c>
+      <c r="D45" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>14</v>
+      </c>
+      <c r="B46" t="n">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" t="s">
+        <v>163</v>
+      </c>
+      <c r="F46" t="s">
+        <v>203</v>
+      </c>
+      <c r="G46" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>14</v>
+      </c>
+      <c r="B47" t="n">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" t="s">
+        <v>202</v>
+      </c>
+      <c r="E47" t="s">
+        <v>163</v>
+      </c>
+      <c r="F47" t="s">
+        <v>203</v>
+      </c>
+      <c r="G47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>14</v>
+      </c>
+      <c r="B48" t="n">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" t="s">
+        <v>202</v>
+      </c>
+      <c r="E48" t="s">
+        <v>163</v>
+      </c>
+      <c r="F48" t="s">
+        <v>203</v>
+      </c>
+      <c r="G48" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>14</v>
+      </c>
+      <c r="B49" t="n">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>202</v>
+      </c>
+      <c r="D49" t="s">
+        <v>202</v>
+      </c>
+      <c r="E49" t="s">
+        <v>163</v>
+      </c>
+      <c r="F49" t="s">
+        <v>203</v>
+      </c>
+      <c r="G49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>14</v>
+      </c>
+      <c r="B50" t="n">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s">
+        <v>202</v>
+      </c>
+      <c r="D50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E50" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" t="s">
+        <v>203</v>
+      </c>
+      <c r="G50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>14</v>
+      </c>
+      <c r="B51" t="n">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51" t="s">
+        <v>163</v>
+      </c>
+      <c r="F51" t="s">
+        <v>203</v>
+      </c>
+      <c r="G51" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>14</v>
+      </c>
+      <c r="B52" t="n">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>202</v>
+      </c>
+      <c r="D52" t="s">
+        <v>202</v>
+      </c>
+      <c r="E52" t="s">
+        <v>163</v>
+      </c>
+      <c r="F52" t="s">
+        <v>203</v>
+      </c>
+      <c r="G52" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>14</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" t="s">
+        <v>202</v>
+      </c>
+      <c r="E53" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" t="s">
+        <v>203</v>
+      </c>
+      <c r="G53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>14</v>
+      </c>
+      <c r="B54" t="n">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" t="s">
+        <v>202</v>
+      </c>
+      <c r="E54" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" t="s">
+        <v>203</v>
+      </c>
+      <c r="G54" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>14</v>
+      </c>
+      <c r="B55" t="n">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>202</v>
+      </c>
+      <c r="D55" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" t="s">
+        <v>203</v>
+      </c>
+      <c r="G55" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>14</v>
+      </c>
+      <c r="B56" t="n">
+        <v>27</v>
+      </c>
+      <c r="C56" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" t="s">
+        <v>202</v>
+      </c>
+      <c r="E56" t="s">
+        <v>163</v>
+      </c>
+      <c r="F56" t="s">
+        <v>203</v>
+      </c>
+      <c r="G56" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>14</v>
+      </c>
+      <c r="B57" t="n">
+        <v>28</v>
+      </c>
+      <c r="C57" t="s">
+        <v>202</v>
+      </c>
+      <c r="D57" t="s">
+        <v>202</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" t="s">
+        <v>203</v>
+      </c>
+      <c r="G57" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>14</v>
+      </c>
+      <c r="B58" t="n">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>202</v>
+      </c>
+      <c r="D58" t="s">
+        <v>202</v>
+      </c>
+      <c r="E58" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58" t="s">
+        <v>203</v>
+      </c>
+      <c r="G58" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>14</v>
+      </c>
+      <c r="B59" t="n">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" t="s">
+        <v>203</v>
+      </c>
+      <c r="G59" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>14</v>
+      </c>
+      <c r="B60" t="n">
+        <v>31</v>
+      </c>
+      <c r="C60" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" t="s">
+        <v>202</v>
+      </c>
+      <c r="E60" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" t="s">
+        <v>203</v>
+      </c>
+      <c r="G60" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2780,7 +3894,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -2796,7 +3910,9 @@
       <c r="D2" t="s">
         <v>207</v>
       </c>
-      <c r="E2"/>
+      <c r="E2" t="s">
+        <v>163</v>
+      </c>
       <c r="F2" t="s">
         <v>208</v>
       </c>
@@ -2817,7 +3933,9 @@
       <c r="D3" t="s">
         <v>212</v>
       </c>
-      <c r="E3"/>
+      <c r="E3" t="s">
+        <v>163</v>
+      </c>
       <c r="F3" t="s">
         <v>213</v>
       </c>
@@ -2838,7 +3956,9 @@
       <c r="D4" t="s">
         <v>217</v>
       </c>
-      <c r="E4"/>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
       <c r="F4" t="s">
         <v>218</v>
       </c>
@@ -2859,11 +3979,15 @@
       <c r="D5" t="s">
         <v>222</v>
       </c>
-      <c r="E5"/>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
       <c r="F5" t="s">
         <v>223</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -2878,11 +4002,15 @@
       <c r="D6" t="s">
         <v>226</v>
       </c>
-      <c r="E6"/>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
       <c r="F6" t="s">
         <v>227</v>
       </c>
-      <c r="G6"/>
+      <c r="G6" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -2897,7 +4025,9 @@
       <c r="D7" t="s">
         <v>230</v>
       </c>
-      <c r="E7"/>
+      <c r="E7" t="s">
+        <v>163</v>
+      </c>
       <c r="F7" t="s">
         <v>231</v>
       </c>
@@ -2918,11 +4048,15 @@
       <c r="D8" t="s">
         <v>235</v>
       </c>
-      <c r="E8"/>
+      <c r="E8" t="s">
+        <v>163</v>
+      </c>
       <c r="F8" t="s">
         <v>236</v>
       </c>
-      <c r="G8"/>
+      <c r="G8" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -2937,7 +4071,9 @@
       <c r="D9" t="s">
         <v>239</v>
       </c>
-      <c r="E9"/>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
       <c r="F9" t="s">
         <v>240</v>
       </c>
@@ -2958,7 +4094,9 @@
       <c r="D10" t="s">
         <v>244</v>
       </c>
-      <c r="E10"/>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
       <c r="F10" t="s">
         <v>245</v>
       </c>
@@ -2979,7 +4117,9 @@
       <c r="D11" t="s">
         <v>249</v>
       </c>
-      <c r="E11"/>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
       <c r="F11" t="s">
         <v>250</v>
       </c>
@@ -3000,11 +4140,15 @@
       <c r="D12" t="s">
         <v>253</v>
       </c>
-      <c r="E12"/>
+      <c r="E12" t="s">
+        <v>163</v>
+      </c>
       <c r="F12" t="s">
         <v>254</v>
       </c>
-      <c r="G12"/>
+      <c r="G12" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -3025,7 +4169,9 @@
       <c r="F13" t="s">
         <v>259</v>
       </c>
-      <c r="G13"/>
+      <c r="G13" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -3040,11 +4186,15 @@
       <c r="D14" t="s">
         <v>261</v>
       </c>
-      <c r="E14"/>
+      <c r="E14" t="s">
+        <v>163</v>
+      </c>
       <c r="F14" t="s">
         <v>262</v>
       </c>
-      <c r="G14"/>
+      <c r="G14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -3059,7 +4209,9 @@
       <c r="D15" t="s">
         <v>265</v>
       </c>
-      <c r="E15"/>
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
       <c r="F15" t="s">
         <v>266</v>
       </c>
@@ -3080,11 +4232,15 @@
       <c r="D16" t="s">
         <v>269</v>
       </c>
-      <c r="E16"/>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
       <c r="F16" t="s">
         <v>270</v>
       </c>
-      <c r="G16"/>
+      <c r="G16" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -3099,7 +4255,9 @@
       <c r="D17" t="s">
         <v>273</v>
       </c>
-      <c r="E17"/>
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
       <c r="F17" t="s">
         <v>274</v>
       </c>
@@ -3120,11 +4278,15 @@
       <c r="D18" t="s">
         <v>278</v>
       </c>
-      <c r="E18"/>
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
       <c r="F18" t="s">
         <v>279</v>
       </c>
-      <c r="G18"/>
+      <c r="G18" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -3162,7 +4324,9 @@
       <c r="D20" t="s">
         <v>288</v>
       </c>
-      <c r="E20"/>
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
       <c r="F20" t="s">
         <v>289</v>
       </c>
@@ -3183,7 +4347,9 @@
       <c r="D21" t="s">
         <v>293</v>
       </c>
-      <c r="E21"/>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
       <c r="F21" t="s">
         <v>294</v>
       </c>
@@ -3204,7 +4370,9 @@
       <c r="D22" t="s">
         <v>298</v>
       </c>
-      <c r="E22"/>
+      <c r="E22" t="s">
+        <v>163</v>
+      </c>
       <c r="F22" t="s">
         <v>299</v>
       </c>
@@ -3225,7 +4393,9 @@
       <c r="D23" t="s">
         <v>302</v>
       </c>
-      <c r="E23"/>
+      <c r="E23" t="s">
+        <v>163</v>
+      </c>
       <c r="F23" t="s">
         <v>303</v>
       </c>
@@ -3246,7 +4416,9 @@
       <c r="D24" t="s">
         <v>307</v>
       </c>
-      <c r="E24"/>
+      <c r="E24" t="s">
+        <v>163</v>
+      </c>
       <c r="F24" t="s">
         <v>308</v>
       </c>
@@ -3267,11 +4439,15 @@
       <c r="D25" t="s">
         <v>311</v>
       </c>
-      <c r="E25"/>
+      <c r="E25" t="s">
+        <v>163</v>
+      </c>
       <c r="F25" t="s">
         <v>312</v>
       </c>
-      <c r="G25"/>
+      <c r="G25" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -3309,11 +4485,15 @@
       <c r="D27" t="s">
         <v>320</v>
       </c>
-      <c r="E27"/>
+      <c r="E27" t="s">
+        <v>163</v>
+      </c>
       <c r="F27" t="s">
         <v>321</v>
       </c>
-      <c r="G27"/>
+      <c r="G27" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -3328,7 +4508,9 @@
       <c r="D28" t="s">
         <v>324</v>
       </c>
-      <c r="E28"/>
+      <c r="E28" t="s">
+        <v>163</v>
+      </c>
       <c r="F28" t="s">
         <v>325</v>
       </c>
@@ -3372,7 +4554,9 @@
       <c r="D30" t="s">
         <v>335</v>
       </c>
-      <c r="E30"/>
+      <c r="E30" t="s">
+        <v>163</v>
+      </c>
       <c r="F30" t="s">
         <v>336</v>
       </c>
@@ -3393,11 +4577,15 @@
       <c r="D31" t="s">
         <v>340</v>
       </c>
-      <c r="E31"/>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
       <c r="F31" t="s">
         <v>341</v>
       </c>
-      <c r="G31"/>
+      <c r="G31" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -3412,11 +4600,15 @@
       <c r="D32" t="s">
         <v>343</v>
       </c>
-      <c r="E32"/>
+      <c r="E32" t="s">
+        <v>163</v>
+      </c>
       <c r="F32" t="s">
         <v>344</v>
       </c>
-      <c r="G32"/>
+      <c r="G32" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -3431,11 +4623,15 @@
       <c r="D33" t="s">
         <v>346</v>
       </c>
-      <c r="E33"/>
+      <c r="E33" t="s">
+        <v>163</v>
+      </c>
       <c r="F33" t="s">
         <v>347</v>
       </c>
-      <c r="G33"/>
+      <c r="G33" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -3450,11 +4646,15 @@
       <c r="D34" t="s">
         <v>350</v>
       </c>
-      <c r="E34"/>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
       <c r="F34" t="s">
         <v>351</v>
       </c>
-      <c r="G34"/>
+      <c r="G34" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -3492,7 +4692,9 @@
       <c r="D36" t="s">
         <v>359</v>
       </c>
-      <c r="E36"/>
+      <c r="E36" t="s">
+        <v>163</v>
+      </c>
       <c r="F36" t="s">
         <v>360</v>
       </c>
@@ -3513,11 +4715,15 @@
       <c r="D37" t="s">
         <v>363</v>
       </c>
-      <c r="E37"/>
+      <c r="E37" t="s">
+        <v>163</v>
+      </c>
       <c r="F37" t="s">
         <v>364</v>
       </c>
-      <c r="G37"/>
+      <c r="G37" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
@@ -3532,11 +4738,15 @@
       <c r="D38" t="s">
         <v>367</v>
       </c>
-      <c r="E38"/>
+      <c r="E38" t="s">
+        <v>163</v>
+      </c>
       <c r="F38" t="s">
         <v>368</v>
       </c>
-      <c r="G38"/>
+      <c r="G38" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
@@ -3580,7 +4790,9 @@
       <c r="F40" t="s">
         <v>379</v>
       </c>
-      <c r="G40"/>
+      <c r="G40" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
@@ -3595,11 +4807,15 @@
       <c r="D41" t="s">
         <v>382</v>
       </c>
-      <c r="E41"/>
+      <c r="E41" t="s">
+        <v>163</v>
+      </c>
       <c r="F41" t="s">
         <v>383</v>
       </c>
-      <c r="G41"/>
+      <c r="G41" t="s">
+        <v>163</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3632,7 +4848,7 @@
         <v>160</v>
       </c>
       <c r="F1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -3648,7 +4864,9 @@
       <c r="D2" t="s">
         <v>386</v>
       </c>
-      <c r="E2"/>
+      <c r="E2" t="s">
+        <v>163</v>
+      </c>
       <c r="F2" t="s">
         <v>387</v>
       </c>
@@ -3666,8 +4884,12 @@
       <c r="D3" t="s">
         <v>390</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
+      <c r="E3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -3682,7 +4904,9 @@
       <c r="D4" t="s">
         <v>393</v>
       </c>
-      <c r="E4"/>
+      <c r="E4" t="s">
+        <v>163</v>
+      </c>
       <c r="F4" t="s">
         <v>394</v>
       </c>
@@ -3700,8 +4924,12 @@
       <c r="D5" t="s">
         <v>396</v>
       </c>
-      <c r="E5"/>
-      <c r="F5"/>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -3716,8 +4944,12 @@
       <c r="D6" t="s">
         <v>398</v>
       </c>
-      <c r="E6"/>
-      <c r="F6"/>
+      <c r="E6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" t="s">
+        <v>163</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>